<commit_message>
Modficacion Curso básico, puntos de extension
</commit_message>
<xml_diff>
--- a/CU04 Realizar Llamada.xlsx
+++ b/CU04 Realizar Llamada.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Revisor</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Paso 5 - El sistema invoca CU ModificarEstadoTicket</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado de la oportunidad. Invocando CU ModificarEstadoOportunidad</t>
+  </si>
+  <si>
+    <t>Paso 6 - El sistema invoca CU ModificarEstadoOportunidad</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,81 +743,97 @@
       <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="B13" s="23"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>2</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
+        <v>2</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>3</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B16" s="26" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>4</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>23</v>
       </c>
       <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
+        <v>5</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>6</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>7</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificacion de los nombres de CU invocados
</commit_message>
<xml_diff>
--- a/CU04 Realizar Llamada.xlsx
+++ b/CU04 Realizar Llamada.xlsx
@@ -130,19 +130,19 @@
     <t>El sistema registrá un nuevo ticket.</t>
   </si>
   <si>
-    <t>El sistema modifica el estado del ticket. Invocando CU ModificarEstadoTicket</t>
-  </si>
-  <si>
     <t>Realizar Llamada</t>
   </si>
   <si>
-    <t>Paso 5 - El sistema invoca CU ModificarEstadoTicket</t>
-  </si>
-  <si>
-    <t>El sistema modifica el estado de la oportunidad. Invocando CU ModificarEstadoOportunidad</t>
-  </si>
-  <si>
-    <t>Paso 6 - El sistema invoca CU ModificarEstadoOportunidad</t>
+    <t>Paso 5 - El sistema invoca CU Cambio Estado Ticket</t>
+  </si>
+  <si>
+    <t>Paso 6 - El sistema invoca CU Cambio Estado Oportunidad</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado del ticket. Invocando CU Cambio Estado Ticket</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado de la oportunidad. Invocando CU Cambio Estado Oportunidad</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="6"/>
@@ -738,14 +738,14 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="28"/>
     </row>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="11"/>
     </row>
@@ -806,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" s="11"/>
     </row>

</xml_diff>

<commit_message>
modifación sobre invocacion a casos de usos
</commit_message>
<xml_diff>
--- a/CU04 Realizar Llamada.xlsx
+++ b/CU04 Realizar Llamada.xlsx
@@ -133,16 +133,16 @@
     <t>Realizar Llamada</t>
   </si>
   <si>
-    <t>Paso 6 - El sistema invoca CU Cambio Estado Oportunidad</t>
-  </si>
-  <si>
-    <t>El sistema modifica el estado de la oportunidad. Invocando CU Cambio Estado Oportunidad</t>
-  </si>
-  <si>
     <t>El sistema modifica el estado del ticket. Invocando CU05 Cambio Estado Ticket</t>
   </si>
   <si>
     <t>Paso 5 - El sistema invoca CU05 Cambio Estado Ticket</t>
+  </si>
+  <si>
+    <t>Paso 6 - El sistema invoca CU06 Cambio Estado Oportunidad</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado de la oportunidad. Invocando CU06 Cambio Estado Oportunidad</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,14 +738,14 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="28"/>
     </row>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="11"/>
     </row>
@@ -806,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="11"/>
     </row>

</xml_diff>

<commit_message>
Eliminadas las invocaciones a CU
</commit_message>
<xml_diff>
--- a/CU04 Realizar Llamada.xlsx
+++ b/CU04 Realizar Llamada.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Revisor</t>
   </si>
@@ -121,18 +121,6 @@
     <t>Realizar Llamada</t>
   </si>
   <si>
-    <t>El sistema modifica el estado del ticket. Invocando CU05 Cambio Estado Ticket</t>
-  </si>
-  <si>
-    <t>Paso 5 - El sistema invoca CU05 Cambio Estado Ticket</t>
-  </si>
-  <si>
-    <t>Paso 6 - El sistema invoca CU06 Cambio Estado Oportunidad</t>
-  </si>
-  <si>
-    <t>El sistema modifica el estado de la oportunidad. Invocando CU06 Cambio Estado Oportunidad</t>
-  </si>
-  <si>
     <t>Que existan campañas activas.
 Que existan oportunidades asignadas a campañas.
 Que existan oportunidades en estado "Abierta"
@@ -144,6 +132,12 @@
   </si>
   <si>
     <t>El sistema muestra en pantalla el formulario "Ticket".</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado del ticket.</t>
+  </si>
+  <si>
+    <t>El sistema modifica el estado de la oportunidad.</t>
   </si>
 </sst>
 </file>
@@ -243,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -317,12 +311,6 @@
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -626,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="12"/>
     </row>
@@ -720,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" s="12"/>
     </row>
@@ -734,104 +722,90 @@
       <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="27"/>
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="27"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>3</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>6</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="10"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>7</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C20" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>